<commit_message>
Changes (Rel.Position, Rel.Depth) to script and ReadMe. Changed directory structure (-> c_script).
</commit_message>
<xml_diff>
--- a/b_output_data_smarttester/descriptivestats_smarttester_stepmm.xlsx
+++ b/b_output_data_smarttester/descriptivestats_smarttester_stepmm.xlsx
@@ -72,22 +72,22 @@
     <t xml:space="preserve">Friction.sd</t>
   </si>
   <si>
-    <t xml:space="preserve">Depth.n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth.min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth.max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth.mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth.median</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth.sd</t>
+    <t xml:space="preserve">Rel.Depth.n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel.Depth.min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel.Depth.max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel.Depth.mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel.Depth.median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel.Depth.sd</t>
   </si>
   <si>
     <t xml:space="preserve">Velocity.n</t>
@@ -627,16 +627,16 @@
         <v>20560</v>
       </c>
       <c r="O2" t="n">
-        <v>1.8775628</v>
+        <v>-3.0199262</v>
       </c>
       <c r="P2" t="n">
-        <v>4.897489</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>4.32427869732004</v>
+        <v>-0.573210302679961</v>
       </c>
       <c r="R2" t="n">
-        <v>4.4065876</v>
+        <v>-0.4909014</v>
       </c>
       <c r="S2" t="n">
         <v>0.381221774101031</v>
@@ -704,16 +704,16 @@
         <v>18581</v>
       </c>
       <c r="O3" t="n">
-        <v>3.973304</v>
+        <v>-3.95333</v>
       </c>
       <c r="P3" t="n">
-        <v>7.926634</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>6.48509117566869</v>
+        <v>-1.44154282433131</v>
       </c>
       <c r="R3" t="n">
-        <v>6.6859365</v>
+        <v>-1.2406975</v>
       </c>
       <c r="S3" t="n">
         <v>0.724268670938382</v>
@@ -781,16 +781,16 @@
         <v>19996</v>
       </c>
       <c r="O4" t="n">
-        <v>4.8475537</v>
+        <v>-0.686801</v>
       </c>
       <c r="P4" t="n">
-        <v>5.5343547</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>5.15189006365273</v>
+        <v>-0.382464636347269</v>
       </c>
       <c r="R4" t="n">
-        <v>5.2869835</v>
+        <v>-0.2473712</v>
       </c>
       <c r="S4" t="n">
         <v>0.176857397678085</v>
@@ -858,16 +858,16 @@
         <v>18591</v>
       </c>
       <c r="O5" t="n">
-        <v>5.4291067</v>
+        <v>-1.481154</v>
       </c>
       <c r="P5" t="n">
-        <v>6.9102607</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>6.09664910628799</v>
+        <v>-0.813611593712011</v>
       </c>
       <c r="R5" t="n">
-        <v>5.9906855</v>
+        <v>-0.919575200000001</v>
       </c>
       <c r="S5" t="n">
         <v>0.433883274541857</v>

</xml_diff>